<commit_message>
completed available handle materials
</commit_message>
<xml_diff>
--- a/Dependencies.xlsx
+++ b/Dependencies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Studium\Semester_03\ComEng\Uebung\Uebung05\CE05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\OneDrive - Johannes Kepler Universität Linz\3.Semester\Communications Engineering\UE\Uebung6\CE05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7021CB6B-0A8E-4085-AB00-7C91714CBE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7021CB6B-0A8E-4085-AB00-7C91714CBE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B876B83A-749C-42A5-A4E5-721AC5E4A242}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{743AA5E5-3C8E-4AB0-B7E6-B189C3C9B539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{743AA5E5-3C8E-4AB0-B7E6-B189C3C9B539}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -449,7 +448,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>